<commit_message>
edi energy mirror cronjob
</commit_message>
<xml_diff>
--- a/edi_energy_de/current/ÄnderungsantragEBD1.2_99991231_20220406.xlsx
+++ b/edi_energy_de/current/ÄnderungsantragEBD1.2_99991231_20220406.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\ER-R\Marktkommunikation\Projektgruppen\PG Entscheidungsbaum-Diagramme\Vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanessa.stemplowsky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AAACB9-49C6-40DB-A79D-945EE7E8849C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35F7B6B-5EEB-486F-B34E-E221223E1339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8EF595F1-0398-4D81-BA29-DB9CB03CA0C4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EF595F1-0398-4D81-BA29-DB9CB03CA0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Einführung" sheetId="1" r:id="rId1"/>
@@ -78,6 +78,1062 @@
     <t>Telefon:</t>
   </si>
   <si>
+    <t>Formblatt für die Übermittlung von  Änderungsanträgen zu den
+Entscheidungsbaum-Diagrammen und Codelisten</t>
+  </si>
+  <si>
+    <t>Dokument</t>
+  </si>
+  <si>
+    <t>Version des Dokumentes</t>
+  </si>
+  <si>
+    <t>Seite</t>
+  </si>
+  <si>
+    <t>Kapitel</t>
+  </si>
+  <si>
+    <t>EBD</t>
+  </si>
+  <si>
+    <t>Bisheriger Inhalt</t>
+  </si>
+  <si>
+    <t>Vorgeschlagene Änderung</t>
+  </si>
+  <si>
+    <t>Herleitung der Änderung</t>
+  </si>
+  <si>
+    <t>Einreicher</t>
+  </si>
+  <si>
+    <t>Entscheidungsbaum-Diagramme und Codelisten</t>
+  </si>
+  <si>
+    <t>E_0400_Kündigung Stromliefervertrag prüfen</t>
+  </si>
+  <si>
+    <t>E_0401_Abmeldung prüfen</t>
+  </si>
+  <si>
+    <t>E_0502_Abmeldung prüfen</t>
+  </si>
+  <si>
+    <t>E_0462_Prüfen, ob Anmeldung direkt ablehnbar</t>
+  </si>
+  <si>
+    <t>E_0403_Abmeldeanfrage prüfen</t>
+  </si>
+  <si>
+    <t>E_0404_Lieferbeginn prüfen</t>
+  </si>
+  <si>
+    <t>E_0456_Lieferschein prüfen</t>
+  </si>
+  <si>
+    <t>E_0503_Rechnung einer sonstigen Leistung prüfen</t>
+  </si>
+  <si>
+    <t>E_0504_Nicht-Zahlungsavis prüfen</t>
+  </si>
+  <si>
+    <t>E_0505_erneut Rechnung einer sonstigen Leistung prüfen</t>
+  </si>
+  <si>
+    <t>E_0506_Prüfen, ob Antwort auf Stornierung erforderlich</t>
+  </si>
+  <si>
+    <t>E_0470_Sperrauftrag prüfen</t>
+  </si>
+  <si>
+    <t>E_0488_Anfrage prüfen</t>
+  </si>
+  <si>
+    <t>E_0501_Ablehnung prüfen, ggf. Clearing durchführen</t>
+  </si>
+  <si>
+    <t>E_0472_Prüfen, ob Sperrauftrag erfolgreich</t>
+  </si>
+  <si>
+    <t>E_0497_Entsperrauftrag prüfen</t>
+  </si>
+  <si>
+    <t>E_0499_Prüfen, ob Entsperrauftrag erfolgreich</t>
+  </si>
+  <si>
+    <t>E_0468_Stornierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0487_Prüfen, ob Entsperrauftrag erfolgreich</t>
+  </si>
+  <si>
+    <t>E_0453_Änderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0455_Information prüfen</t>
+  </si>
+  <si>
+    <t>E_0476_Reklamation prüfen</t>
+  </si>
+  <si>
+    <t>E_0478_Reklamation prüfen</t>
+  </si>
+  <si>
+    <t>E_0479_Reklamation prüfen</t>
+  </si>
+  <si>
+    <t>E_0483_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0484_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0493_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0485_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0494_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0486_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0495_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0480_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0496_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0481_Bestellanforderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0482_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0492 Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0474_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0490 Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0475_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0491_ Prüfen, ob Parametrierung für betroffene Messlokation durchgeführt werden konnte</t>
+  </si>
+  <si>
+    <t>E_0477_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0441_Geschäftsdatenanfrage zu Stammdaten prüfen</t>
+  </si>
+  <si>
+    <t>E_0442_Geschäftsdatenanfrage zu Werten prüfen</t>
+  </si>
+  <si>
+    <t>E_0443_Geschäftsdatenanfrage zu Stammdaten prüfen</t>
+  </si>
+  <si>
+    <t>E_0444_Geschäftsdatenanfrage zu Werten prüfe</t>
+  </si>
+  <si>
+    <t>E_0020_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0024_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0010_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0009_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0040_NZR prüfen</t>
+  </si>
+  <si>
+    <t>E_0008_NZR prüfen</t>
+  </si>
+  <si>
+    <t>E_0066_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
+  </si>
+  <si>
+    <t>E_0067_Datenstatus nach Eingang einer Netzzeitreihe vergeben</t>
+  </si>
+  <si>
+    <t>E_0100 Profile bzw. Profilscharen prüfen</t>
+  </si>
+  <si>
+    <t>E_0101 normierte synthetische SLP prüfen</t>
+  </si>
+  <si>
+    <t>E_0007_LF-SZR (Kategorie A) prüfen</t>
+  </si>
+  <si>
+    <t>E_0047_Marktlokationen mit LF-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0049_Marktlokationen mit LF-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0041_Lieferantensummenzeitreihe (Kategorie B) prüfen</t>
+  </si>
+  <si>
+    <t>E_0014_Marktlokationen mit LF-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0004_Marktlokationen mit LF-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0015_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0035_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0017_Marktlokationen mit BG-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0052_Marktlokationen mit BG-CL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0036_Bilanzierungsgebietssummenzeitreihe (Kategorie B) prüfen</t>
+  </si>
+  <si>
+    <t>E_0062_BG-SZR (Kategorie B) prüfen</t>
+  </si>
+  <si>
+    <t>E_0019_Prüfmitteilung prüfen</t>
+  </si>
+  <si>
+    <t>E_0053_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
+  </si>
+  <si>
+    <t>E_0054_Datenstatus nach Eingang einer Bilanzierungsgebietssummenzeitreihe (Kategorie B) vergeben</t>
+  </si>
+  <si>
+    <t>E_0055_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
+  </si>
+  <si>
+    <t>E_0034_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0018_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0068_Einzelanforderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0038_Bilanzkreissummenzeitreihe (Kategorie A) prüfen</t>
+  </si>
+  <si>
+    <t>E_0063_BK-SZR (Kategorie A) prüfen</t>
+  </si>
+  <si>
+    <t>E_0021_Prüfmitteilung prüfen</t>
+  </si>
+  <si>
+    <t>E_0056_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
+  </si>
+  <si>
+    <t>E_0057_Datenstatus nach Eingang einer Bilanzkreissummenzeitreihe (Kategorie A) vergeben</t>
+  </si>
+  <si>
+    <t>E_0058_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
+  </si>
+  <si>
+    <t>E_0011_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0012_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0039_Einzelanforderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0022_Abbestellung der Aggregationsebene RZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0003_Bestellung der Aggregationsebene RZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0023_Bilanzkreissummenzeitreihe (Kategorie B) prüfen</t>
+  </si>
+  <si>
+    <t>E_0064_BK_SZR (Kategorie B) prüfen</t>
+  </si>
+  <si>
+    <t>E_0025_Prüfmitteilung prüfen</t>
+  </si>
+  <si>
+    <t>E_0026_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
+  </si>
+  <si>
+    <t>E_0042_Datenstatus nach Eingang einer Bilanzkreissummenzeitreihe (Kategorie B) vergeben</t>
+  </si>
+  <si>
+    <t>E_0043_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
+  </si>
+  <si>
+    <t>E_0027_MaBiS-ZP Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0028_MaBiS-ZP Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0070_DZÜ-Liste prüfen</t>
+  </si>
+  <si>
+    <t>E_0029_Deltazeitreihenübertrag prüfen</t>
+  </si>
+  <si>
+    <t>E_0065_DZÜ prüfen</t>
+  </si>
+  <si>
+    <t>E_0030_Prüfmitteilung prüfen</t>
+  </si>
+  <si>
+    <t>E_0059_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
+  </si>
+  <si>
+    <t>E_0060_Datenstatus nach Eingang eines Deltazeitreihenübertrags vergeben</t>
+  </si>
+  <si>
+    <t>E_0061_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
+  </si>
+  <si>
+    <t>E_0093_LF-AASZR prüfen</t>
+  </si>
+  <si>
+    <t>E_0096_Marktlokationen mit LF-AACL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0097_Marktlokationen mit LF-AACL abgleichen</t>
+  </si>
+  <si>
+    <t>E_0071_MaBiS-ZP AAÜZ Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0072_MaBiS-ZP AAÜZ Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0073_AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0098_monatliche AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0074_Prüfmitteilung AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0075_Datenstatus AAÜZ nach erfolgter BKA vergeben</t>
+  </si>
+  <si>
+    <t>E_0076_Datenstatus nach Eingang einer AAÜZ vergeben</t>
+  </si>
+  <si>
+    <t>E_0077_Datenstatus nach Vorliegen einer Prüfmitteilung zur AAÜZ vergeben</t>
+  </si>
+  <si>
+    <t>E_0078_MaBiS-ZP AAÜZ Aktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0079_MaBiS-ZP AAÜZ Deaktivierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0080_AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0099_monatliche AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0081_Prüfmitteilung AAÜZ prüfen</t>
+  </si>
+  <si>
+    <t>E_0082_Datenstatus AAÜZ nach erfolgter BKA vergeben</t>
+  </si>
+  <si>
+    <t>E_0083_Datenstatus nach Eingang einer AAÜZ vergeben</t>
+  </si>
+  <si>
+    <t>E_0084_Datenstatus nach Vorliegen einer Prüfmitteilung zur AAÜZ vergeben</t>
+  </si>
+  <si>
+    <t>E_0302_Abmeldung prüfen</t>
+  </si>
+  <si>
+    <t>E_0249_Beauftragung zur Messlokationsänderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0250_Beauftragung zur Messlokationsänderung prüfen</t>
+  </si>
+  <si>
+    <t>E_0233_Prüfung Selbsteinbau oder Bestandsschutz nach §19 Abs. 5 MsbG</t>
+  </si>
+  <si>
+    <t>E_0205_Angebot prüfen</t>
+  </si>
+  <si>
+    <t>E_0206_Beendigung prüfen</t>
+  </si>
+  <si>
+    <t>E_0207_Anfrage prüfen</t>
+  </si>
+  <si>
+    <t>E_0208_Angebot bzw. Ablehnung der Anfrage verarbeiten</t>
+  </si>
+  <si>
+    <t>E_0209_Beendigung prüfen</t>
+  </si>
+  <si>
+    <t>E_0218_Berechnungsformel prüfen</t>
+  </si>
+  <si>
+    <t>E_0252_Anfrage prüfen</t>
+  </si>
+  <si>
+    <t>E_0256_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0257_Stornierung prüfen</t>
+  </si>
+  <si>
+    <t>E_0254_Beendigung prüfen</t>
+  </si>
+  <si>
+    <t>E_0800_Bestellung prüfen</t>
+  </si>
+  <si>
+    <t>E_0900_Prüfung der Ausfallarbeit</t>
+  </si>
+  <si>
+    <t>E_0901_Gegenvorschlag prüfen</t>
+  </si>
+  <si>
+    <t>E_0902_Ausfallarbeit unter Einbeziehung Fahrplananteil plausibilisieren</t>
+  </si>
+  <si>
+    <t>E_0903_Antwort verarbeiten</t>
+  </si>
+  <si>
+    <t>sonstiges</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>4.2 SD: Stammdatensynchronisation</t>
+  </si>
+  <si>
+    <t>Beispiel für die Ausfüllung des Formulars</t>
+  </si>
+  <si>
+    <t>BDEW</t>
+  </si>
+  <si>
+    <t>[…]
+Nr. 22
+Prüfschritt
+Entspricht das Bilanzierungsverfahren dem gültigen Bilanzierungsverfahren zur Datenaggregation beim ÜNB?
+Prüfergebnis 
+ja -&gt; 23
+nein -&gt; 23 Code A09
+Hinweis
+Bilanzierungsverfahren nicht gültig
+Nr. 23
+Prüfschritt
+Wird die Marktlokation auf grundlage von profilen bilanziert?
+Prüfergebnis
+ja -&gt; 24
+nein -&gt;27
+Nr. 24
+Prüfschritt
+Ist das angegebene normierte Profil zum angegebenen Zeitpunkt für das Bilanzierungsgebiet Bestandteil der Profildefinitionsliste des Netzbetreibers?
+Prüfergebnis 
+ja -&gt; 25
+nein -&gt; 25 Code A10
+Hinweis
+Normiertes Profil liegt nicht vor</t>
+  </si>
+  <si>
+    <t>[…]
+Nr. 22
+Prüfschritt
+Entspricht das Bilanzierungsverfahren dem gültigen Bilanzierungsverfahren zur Datenaggregation beim ÜNB?
+Prüfergebnis 
+ja -&gt; 23
+nein -&gt; 23 Code A09
+Hinweis
+Bilanzierungsverfahren nicht gültig
+Nr. 23
+Prüfschritt
+Ist das angegebene normierte Profil zum angegebenen Zeitpunkt für das Bilanzierungsgebiet Bestandteil der Profildefinitionsliste des Netzbetreibers?
+Prüfergebnis 
+ja -&gt; 25
+nein -&gt; 25 Code A10
+Hinweis
+Normiertes Profil liegt nicht vor</t>
+  </si>
+  <si>
+    <t>Die neue Frage (23) ist erforderlich, damit die nächsten Fragen in der richtigen Reihenfolge erfolgen.</t>
+  </si>
+  <si>
+    <t>E_0104_Listeninhalt prüfen</t>
+  </si>
+  <si>
+    <t>E_0105_Listeninhalt prüfen</t>
+  </si>
+  <si>
+    <t>E_0406_Netznutzungsrechnung prüfen</t>
+  </si>
+  <si>
+    <t>E_0407_erneut Netznutzungsabrechnung prüfen</t>
+  </si>
+  <si>
+    <t>E_0450_Information prüfen</t>
+  </si>
+  <si>
+    <t>E_0459_Prüfen, ob Antwort auf Stornierung erforderlich</t>
+  </si>
+  <si>
+    <t>G_0001_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>G_0002_Antwort auf Änderungsmeldung zur Zuordnungsliste-Gas</t>
+  </si>
+  <si>
+    <t>G_0003_Ablehnung Anfrage Stornierung</t>
+  </si>
+  <si>
+    <t>G_0004_Bestätigung Anfrage Stornierung</t>
+  </si>
+  <si>
+    <t>G_0005_Ablehnung Kündigung</t>
+  </si>
+  <si>
+    <t>G_0006_Bestätigung Kündigung</t>
+  </si>
+  <si>
+    <t>G_0007_Ablehnung Abmeldung</t>
+  </si>
+  <si>
+    <t>G_0008_Bestätigung Abmeldung</t>
+  </si>
+  <si>
+    <t>G_0009_Ablehnung Abmeldungsanfrage</t>
+  </si>
+  <si>
+    <t>G_0010_Bestätigung Abmeldungsanfrage</t>
+  </si>
+  <si>
+    <t>G_0011_Ablehnung der Anmeldung</t>
+  </si>
+  <si>
+    <t>G_0012_Bestätigung der Anmeldung</t>
+  </si>
+  <si>
+    <t>G_0013_Bestätigung EOG Anmeldung</t>
+  </si>
+  <si>
+    <t>G_0014_Ablehnung EOG Anmeldung</t>
+  </si>
+  <si>
+    <t>G_0015_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>G_0016_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>G_0017_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>G_0018_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>G_0019_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>G_0022_Antwort auf Änderung der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>G_0023_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>G_0024_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>G_0025_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>G_0026_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>G_0027_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>G_0029_Antwort auf Änderung</t>
+  </si>
+  <si>
+    <t>G_0030_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>G_0031_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0032_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0033_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>G_0034_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0035_Antwort auf Anfrage der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>G_0036_Ablehnung der Anfrage der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>G_0038_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0039_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>G_0040_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0042_Ablehnung Anfrage</t>
+  </si>
+  <si>
+    <t>G_0043_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0044_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0045_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0046_Ablehnung Anfrage</t>
+  </si>
+  <si>
+    <t>G_0047_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0048_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>G_0049_ORDRSP_Ablehnung der Anforderung von Stammdaten</t>
+  </si>
+  <si>
+    <t>G_0050_ORDRSP_Ablehnung der Anforderung von Messwerten</t>
+  </si>
+  <si>
+    <t>G_0051_Ablehnung Kündigung MSB</t>
+  </si>
+  <si>
+    <t>G_0052_Bestätigung Kündigung MSB</t>
+  </si>
+  <si>
+    <t>G_0053_Ablehnung Anmeldung MSB</t>
+  </si>
+  <si>
+    <t>G_0054_Bestätigung Anmeldung MSB</t>
+  </si>
+  <si>
+    <t>G_0055_Statusmeldung</t>
+  </si>
+  <si>
+    <t>G_0057_Ablehnung Ende MSB</t>
+  </si>
+  <si>
+    <t>G_0058_Bestätigung Ende MSB</t>
+  </si>
+  <si>
+    <t>G_0059_Ankündigung zum Eigenausbau</t>
+  </si>
+  <si>
+    <t>G_0060_Mitteilung, kein Eigenausbau MSBA</t>
+  </si>
+  <si>
+    <t>G_0061_ORDRSP Bestellbestätigung</t>
+  </si>
+  <si>
+    <t>G_0062_ORDRSP Ablehnung der Änderung an LF</t>
+  </si>
+  <si>
+    <t>G_0063_ORDRSP Ablehnung der Änderung an NB</t>
+  </si>
+  <si>
+    <t>G_0064_ORDRSP Auftragsbestätigung an LF</t>
+  </si>
+  <si>
+    <t>G_0065_ORDRSP Auftragsbestätigung an NB</t>
+  </si>
+  <si>
+    <t>G_0066_ORDRSP Ablehnung der Reklamation</t>
+  </si>
+  <si>
+    <t>G_0067_Bestätigung Abmeldung von NB</t>
+  </si>
+  <si>
+    <t>G_0068_Ablehnung Abmeldung von NB</t>
+  </si>
+  <si>
+    <t>G_0069_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>G_0070_Bestätigung Verpflichtungsanfrage</t>
+  </si>
+  <si>
+    <t>G_0071_Ablehnung Verpflichtungsanfrage</t>
+  </si>
+  <si>
+    <t>G_0072_ORDRSP Fortführungsbestätigung MSBA</t>
+  </si>
+  <si>
+    <t>G_0073_ORDRSP Ablehnung</t>
+  </si>
+  <si>
+    <t>G_0074_ORDRSP Ablehnung der Bestellung</t>
+  </si>
+  <si>
+    <t>G_0075_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>G_0076_ORDRSP Mitteilung einer gescheiterten Ablesung</t>
+  </si>
+  <si>
+    <t>G_0077_Mitteilung einer gescheiterten Ablesung</t>
+  </si>
+  <si>
+    <t>G_0078_ORDRSP_Ablehnung der Anforderung</t>
+  </si>
+  <si>
+    <t>G_0079_ Kapazitätsrechnung prüfen</t>
+  </si>
+  <si>
+    <t>G_0080_aggregierte Menge und Abrechnungszeitraum prüfen</t>
+  </si>
+  <si>
+    <t>G_0081_Netznutzungsrechnung prüfen</t>
+  </si>
+  <si>
+    <t>G_0082_ORDRSP_Ablehnung der Anforderung von Messwerten</t>
+  </si>
+  <si>
+    <t>G_0083_Ablehnung der Rechnung vom NB an den MSBA</t>
+  </si>
+  <si>
+    <t>G_0084_Ablehnung der Rechnung vom MSBN an den MSBA</t>
+  </si>
+  <si>
+    <t>G_0085_Ablehnung der Stornorechnung</t>
+  </si>
+  <si>
+    <t>G_0086_Ablehnung der Stornorechnung</t>
+  </si>
+  <si>
+    <t>G_0087_Ablehnung der Stornorechnung</t>
+  </si>
+  <si>
+    <t>G_0088_Ablehnung der Stornorechnung (MMMA NB an MGV)</t>
+  </si>
+  <si>
+    <t>GS_001_Ablehnung auf Stammdaten zur verbrauchenden Marktlokation</t>
+  </si>
+  <si>
+    <t>GS_002_MehrMinderMengen-Rechnung prüfen</t>
+  </si>
+  <si>
+    <t>GS_004_Ablehnung der Stornorechnung (aus Prozessschritt 5 MMMA NB an LF)</t>
+  </si>
+  <si>
+    <t>GS_005_Ablehnung der Stornorechnung (aus Prozessschritt 7 MMMA NB an LF)</t>
+  </si>
+  <si>
+    <t>S_0003_Bestätigung EOG Anmeldung</t>
+  </si>
+  <si>
+    <t>S_0004_Ablehnung EOG Anmeldung</t>
+  </si>
+  <si>
+    <t>S_0005_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0006_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0007_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0008_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0009_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0010_Antwort auf Änderung vom NB</t>
+  </si>
+  <si>
+    <t>S_0013_Antwort auf Änderung der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>S_0014_Antwort auf Änderung der Lokationsbündelstruktur</t>
+  </si>
+  <si>
+    <t>S_0015_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>S_0016_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>S_0017_Antwort auf Änderung vom LF</t>
+  </si>
+  <si>
+    <t>S_0018_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>S_0019_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>S_0020_Antwort auf Änderung vom MSB</t>
+  </si>
+  <si>
+    <t>S_0021_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0022_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0023_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0024_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>S_0025_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0026_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0027_Ablehnung der Anfrage der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>S_0028_Antwort auf Anfrage der Lokationsbündelstruktur</t>
+  </si>
+  <si>
+    <t>S_0029_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0030_Ablehnung Anfrage</t>
+  </si>
+  <si>
+    <t>S_0031_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0032_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0033_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>S_0034_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0035_Ablehnung Anfrage</t>
+  </si>
+  <si>
+    <t>S_0036_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0037_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>S_0038_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0039_Antwort auf Änderung</t>
+  </si>
+  <si>
+    <t>S_0040_Antwort auf Änderung</t>
+  </si>
+  <si>
+    <t>S_0041_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0043_ORDRSP_Ablehnung der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0044_ORDRSP_Ablehnung der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0045_Bestätigung Kündigung</t>
+  </si>
+  <si>
+    <t>S_0046_Ablehnung Kündigung</t>
+  </si>
+  <si>
+    <t>S_0047_Bestätigung Abmeldungsanfrage</t>
+  </si>
+  <si>
+    <t>S_0048_Ablehnung Abmeldungsanfrage</t>
+  </si>
+  <si>
+    <t>S_0049_Bestätigung Anmeldung</t>
+  </si>
+  <si>
+    <t>S_0050_Bestätigung Anmeldung Neuanl. u. LW m. Trbild. b. N-EE+N-KWKG</t>
+  </si>
+  <si>
+    <t>S_0051_Ablehnung Anmeldung</t>
+  </si>
+  <si>
+    <t>S_0052_Ablehnung Abmeldung</t>
+  </si>
+  <si>
+    <t>S_0054_Ablehnung Kündigung MSB</t>
+  </si>
+  <si>
+    <t>S_0055_Bestätigung Anmeldung MSB</t>
+  </si>
+  <si>
+    <t>S_0056_Ablehnung Anmeldung MSB</t>
+  </si>
+  <si>
+    <t>S_0057_Statusmeldung</t>
+  </si>
+  <si>
+    <t>S_0059_Bestätigung Ende MSB</t>
+  </si>
+  <si>
+    <t>S_0060_Ablehnung Ende MSB</t>
+  </si>
+  <si>
+    <t>S_0061_ORDRSP Fortführungsbestätigung MSBA</t>
+  </si>
+  <si>
+    <t>S_0062_ORDRSP Ablehnung</t>
+  </si>
+  <si>
+    <t>S_0063_Bestätigung Verpflichtungsanfrage</t>
+  </si>
+  <si>
+    <t>S_0064_Ablehnung Verpflichtungsanfrage</t>
+  </si>
+  <si>
+    <t>S_0065_Ankündigung zum Eigenausbau</t>
+  </si>
+  <si>
+    <t>S_0066_Mitteilung, kein Eigenausbau MSBA</t>
+  </si>
+  <si>
+    <t>S_0067_ORDRSP Bestellbestätigung</t>
+  </si>
+  <si>
+    <t>S_0068_ORDRSP Abl. der Bestellung</t>
+  </si>
+  <si>
+    <t>S_0073_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0074_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0075_ORDRSP Abl. der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0076_ORDRSP Ablehnung der Reklamation</t>
+  </si>
+  <si>
+    <t>S_0077_ORDRSP Ablehnung der Reklamation</t>
+  </si>
+  <si>
+    <t>S_0078_ORDRSP Ablehnung der Reklamation</t>
+  </si>
+  <si>
+    <t>S_0079_ORDRSP Ablehnung der Reklamation</t>
+  </si>
+  <si>
+    <t>S_0080_Ablehnung auf Stammdaten zur erzeugenden Marktlokation</t>
+  </si>
+  <si>
+    <t>S_0086_Bestätigung Anfrage Stornierung</t>
+  </si>
+  <si>
+    <t>S_0087_Ablehnung Anfrage Stornierung</t>
+  </si>
+  <si>
+    <t>S_0088_Bestätigung Abmeldung</t>
+  </si>
+  <si>
+    <t>S_0090_Bestätigung Kündigung MSBS</t>
+  </si>
+  <si>
+    <t>S_0091_Antwort auf Stammdatenänderung</t>
+  </si>
+  <si>
+    <t>S_0092_ORDRSP Ablehnung der Anforderung</t>
+  </si>
+  <si>
+    <t>S_0093_ORDRSP Bestätigung der Anforderung zum Beenden des Abos zur Stammdaten- bzw. Messwertübermittlung</t>
+  </si>
+  <si>
+    <t>S_0094_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0098_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>S_0099_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0100_Ablehnung der Anfrage</t>
+  </si>
+  <si>
+    <t>S_0101_Antwort auf Anfrage der Marktlokationsstruktur</t>
+  </si>
+  <si>
+    <t>S_0102_Antwort auf Anfrage</t>
+  </si>
+  <si>
+    <t>S_0103_Netznutzungsrechnung prüfen</t>
+  </si>
+  <si>
+    <t>S_0104_erneut Netznutzungsrechnung prüfen</t>
+  </si>
+  <si>
+    <t>S_0106_ Rechnung verarbeiten</t>
+  </si>
+  <si>
+    <t>S_0107_Abrechnung von Dienstleistungen</t>
+  </si>
+  <si>
+    <t>S_0108_Weitere Bearbeitung prüfen</t>
+  </si>
+  <si>
+    <t>S_0109_Nichtzahlungsavis prüfen</t>
+  </si>
+  <si>
+    <t>S_0110_Prüfen, ob Antwort auf Stornierung erforderlich</t>
+  </si>
+  <si>
+    <t>S_0111_Prüfen, ob Antwort auf Stornierung erforderlich</t>
+  </si>
+  <si>
     <r>
       <t>Hinweis:</t>
     </r>
@@ -106,7 +1162,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>clara.gladen@bdew.de</t>
+      <t>vanessa.stemplowsky@bdew.de</t>
     </r>
     <r>
       <rPr>
@@ -120,1062 +1176,6 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>Formblatt für die Übermittlung von  Änderungsanträgen zu den
-Entscheidungsbaum-Diagrammen und Codelisten</t>
-  </si>
-  <si>
-    <t>Dokument</t>
-  </si>
-  <si>
-    <t>Version des Dokumentes</t>
-  </si>
-  <si>
-    <t>Seite</t>
-  </si>
-  <si>
-    <t>Kapitel</t>
-  </si>
-  <si>
-    <t>EBD</t>
-  </si>
-  <si>
-    <t>Bisheriger Inhalt</t>
-  </si>
-  <si>
-    <t>Vorgeschlagene Änderung</t>
-  </si>
-  <si>
-    <t>Herleitung der Änderung</t>
-  </si>
-  <si>
-    <t>Einreicher</t>
-  </si>
-  <si>
-    <t>Entscheidungsbaum-Diagramme und Codelisten</t>
-  </si>
-  <si>
-    <t>E_0400_Kündigung Stromliefervertrag prüfen</t>
-  </si>
-  <si>
-    <t>E_0401_Abmeldung prüfen</t>
-  </si>
-  <si>
-    <t>E_0502_Abmeldung prüfen</t>
-  </si>
-  <si>
-    <t>E_0462_Prüfen, ob Anmeldung direkt ablehnbar</t>
-  </si>
-  <si>
-    <t>E_0403_Abmeldeanfrage prüfen</t>
-  </si>
-  <si>
-    <t>E_0404_Lieferbeginn prüfen</t>
-  </si>
-  <si>
-    <t>E_0456_Lieferschein prüfen</t>
-  </si>
-  <si>
-    <t>E_0503_Rechnung einer sonstigen Leistung prüfen</t>
-  </si>
-  <si>
-    <t>E_0504_Nicht-Zahlungsavis prüfen</t>
-  </si>
-  <si>
-    <t>E_0505_erneut Rechnung einer sonstigen Leistung prüfen</t>
-  </si>
-  <si>
-    <t>E_0506_Prüfen, ob Antwort auf Stornierung erforderlich</t>
-  </si>
-  <si>
-    <t>E_0470_Sperrauftrag prüfen</t>
-  </si>
-  <si>
-    <t>E_0488_Anfrage prüfen</t>
-  </si>
-  <si>
-    <t>E_0501_Ablehnung prüfen, ggf. Clearing durchführen</t>
-  </si>
-  <si>
-    <t>E_0472_Prüfen, ob Sperrauftrag erfolgreich</t>
-  </si>
-  <si>
-    <t>E_0497_Entsperrauftrag prüfen</t>
-  </si>
-  <si>
-    <t>E_0499_Prüfen, ob Entsperrauftrag erfolgreich</t>
-  </si>
-  <si>
-    <t>E_0468_Stornierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0487_Prüfen, ob Entsperrauftrag erfolgreich</t>
-  </si>
-  <si>
-    <t>E_0453_Änderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0455_Information prüfen</t>
-  </si>
-  <si>
-    <t>E_0476_Reklamation prüfen</t>
-  </si>
-  <si>
-    <t>E_0478_Reklamation prüfen</t>
-  </si>
-  <si>
-    <t>E_0479_Reklamation prüfen</t>
-  </si>
-  <si>
-    <t>E_0483_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0484_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0493_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0485_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0494_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0486_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0495_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0480_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0496_Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0481_Bestellanforderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0482_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0492 Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0474_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0490 Prüfen, ob Parametrierung für alle betroffenen Messlokationen durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0475_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0491_ Prüfen, ob Parametrierung für betroffene Messlokation durchgeführt werden konnte</t>
-  </si>
-  <si>
-    <t>E_0477_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0441_Geschäftsdatenanfrage zu Stammdaten prüfen</t>
-  </si>
-  <si>
-    <t>E_0442_Geschäftsdatenanfrage zu Werten prüfen</t>
-  </si>
-  <si>
-    <t>E_0443_Geschäftsdatenanfrage zu Stammdaten prüfen</t>
-  </si>
-  <si>
-    <t>E_0444_Geschäftsdatenanfrage zu Werten prüfe</t>
-  </si>
-  <si>
-    <t>E_0020_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0024_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0010_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0009_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0040_NZR prüfen</t>
-  </si>
-  <si>
-    <t>E_0008_NZR prüfen</t>
-  </si>
-  <si>
-    <t>E_0066_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
-  </si>
-  <si>
-    <t>E_0067_Datenstatus nach Eingang einer Netzzeitreihe vergeben</t>
-  </si>
-  <si>
-    <t>E_0100 Profile bzw. Profilscharen prüfen</t>
-  </si>
-  <si>
-    <t>E_0101 normierte synthetische SLP prüfen</t>
-  </si>
-  <si>
-    <t>E_0007_LF-SZR (Kategorie A) prüfen</t>
-  </si>
-  <si>
-    <t>E_0047_Marktlokationen mit LF-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0049_Marktlokationen mit LF-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0041_Lieferantensummenzeitreihe (Kategorie B) prüfen</t>
-  </si>
-  <si>
-    <t>E_0014_Marktlokationen mit LF-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0004_Marktlokationen mit LF-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0015_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0035_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0017_Marktlokationen mit BG-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0052_Marktlokationen mit BG-CL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0036_Bilanzierungsgebietssummenzeitreihe (Kategorie B) prüfen</t>
-  </si>
-  <si>
-    <t>E_0062_BG-SZR (Kategorie B) prüfen</t>
-  </si>
-  <si>
-    <t>E_0019_Prüfmitteilung prüfen</t>
-  </si>
-  <si>
-    <t>E_0053_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
-  </si>
-  <si>
-    <t>E_0054_Datenstatus nach Eingang einer Bilanzierungsgebietssummenzeitreihe (Kategorie B) vergeben</t>
-  </si>
-  <si>
-    <t>E_0055_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
-  </si>
-  <si>
-    <t>E_0034_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0018_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0068_Einzelanforderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0038_Bilanzkreissummenzeitreihe (Kategorie A) prüfen</t>
-  </si>
-  <si>
-    <t>E_0063_BK-SZR (Kategorie A) prüfen</t>
-  </si>
-  <si>
-    <t>E_0021_Prüfmitteilung prüfen</t>
-  </si>
-  <si>
-    <t>E_0056_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
-  </si>
-  <si>
-    <t>E_0057_Datenstatus nach Eingang einer Bilanzkreissummenzeitreihe (Kategorie A) vergeben</t>
-  </si>
-  <si>
-    <t>E_0058_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
-  </si>
-  <si>
-    <t>E_0011_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0012_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0039_Einzelanforderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0022_Abbestellung der Aggregationsebene RZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0003_Bestellung der Aggregationsebene RZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0023_Bilanzkreissummenzeitreihe (Kategorie B) prüfen</t>
-  </si>
-  <si>
-    <t>E_0064_BK_SZR (Kategorie B) prüfen</t>
-  </si>
-  <si>
-    <t>E_0025_Prüfmitteilung prüfen</t>
-  </si>
-  <si>
-    <t>E_0026_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
-  </si>
-  <si>
-    <t>E_0042_Datenstatus nach Eingang einer Bilanzkreissummenzeitreihe (Kategorie B) vergeben</t>
-  </si>
-  <si>
-    <t>E_0043_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
-  </si>
-  <si>
-    <t>E_0027_MaBiS-ZP Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0028_MaBiS-ZP Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0070_DZÜ-Liste prüfen</t>
-  </si>
-  <si>
-    <t>E_0029_Deltazeitreihenübertrag prüfen</t>
-  </si>
-  <si>
-    <t>E_0065_DZÜ prüfen</t>
-  </si>
-  <si>
-    <t>E_0030_Prüfmitteilung prüfen</t>
-  </si>
-  <si>
-    <t>E_0059_Datenstatus nach erfolgter Bilanzkreisabrechnung vergeben</t>
-  </si>
-  <si>
-    <t>E_0060_Datenstatus nach Eingang eines Deltazeitreihenübertrags vergeben</t>
-  </si>
-  <si>
-    <t>E_0061_Datenstatus nach Vorliegen einer Prüfmitteilung vergeben</t>
-  </si>
-  <si>
-    <t>E_0093_LF-AASZR prüfen</t>
-  </si>
-  <si>
-    <t>E_0096_Marktlokationen mit LF-AACL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0097_Marktlokationen mit LF-AACL abgleichen</t>
-  </si>
-  <si>
-    <t>E_0071_MaBiS-ZP AAÜZ Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0072_MaBiS-ZP AAÜZ Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0073_AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0098_monatliche AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0074_Prüfmitteilung AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0075_Datenstatus AAÜZ nach erfolgter BKA vergeben</t>
-  </si>
-  <si>
-    <t>E_0076_Datenstatus nach Eingang einer AAÜZ vergeben</t>
-  </si>
-  <si>
-    <t>E_0077_Datenstatus nach Vorliegen einer Prüfmitteilung zur AAÜZ vergeben</t>
-  </si>
-  <si>
-    <t>E_0078_MaBiS-ZP AAÜZ Aktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0079_MaBiS-ZP AAÜZ Deaktivierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0080_AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0099_monatliche AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0081_Prüfmitteilung AAÜZ prüfen</t>
-  </si>
-  <si>
-    <t>E_0082_Datenstatus AAÜZ nach erfolgter BKA vergeben</t>
-  </si>
-  <si>
-    <t>E_0083_Datenstatus nach Eingang einer AAÜZ vergeben</t>
-  </si>
-  <si>
-    <t>E_0084_Datenstatus nach Vorliegen einer Prüfmitteilung zur AAÜZ vergeben</t>
-  </si>
-  <si>
-    <t>E_0302_Abmeldung prüfen</t>
-  </si>
-  <si>
-    <t>E_0249_Beauftragung zur Messlokationsänderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0250_Beauftragung zur Messlokationsänderung prüfen</t>
-  </si>
-  <si>
-    <t>E_0233_Prüfung Selbsteinbau oder Bestandsschutz nach §19 Abs. 5 MsbG</t>
-  </si>
-  <si>
-    <t>E_0205_Angebot prüfen</t>
-  </si>
-  <si>
-    <t>E_0206_Beendigung prüfen</t>
-  </si>
-  <si>
-    <t>E_0207_Anfrage prüfen</t>
-  </si>
-  <si>
-    <t>E_0208_Angebot bzw. Ablehnung der Anfrage verarbeiten</t>
-  </si>
-  <si>
-    <t>E_0209_Beendigung prüfen</t>
-  </si>
-  <si>
-    <t>E_0218_Berechnungsformel prüfen</t>
-  </si>
-  <si>
-    <t>E_0252_Anfrage prüfen</t>
-  </si>
-  <si>
-    <t>E_0256_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0257_Stornierung prüfen</t>
-  </si>
-  <si>
-    <t>E_0254_Beendigung prüfen</t>
-  </si>
-  <si>
-    <t>E_0800_Bestellung prüfen</t>
-  </si>
-  <si>
-    <t>E_0900_Prüfung der Ausfallarbeit</t>
-  </si>
-  <si>
-    <t>E_0901_Gegenvorschlag prüfen</t>
-  </si>
-  <si>
-    <t>E_0902_Ausfallarbeit unter Einbeziehung Fahrplananteil plausibilisieren</t>
-  </si>
-  <si>
-    <t>E_0903_Antwort verarbeiten</t>
-  </si>
-  <si>
-    <t>sonstiges</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>4.2 SD: Stammdatensynchronisation</t>
-  </si>
-  <si>
-    <t>Beispiel für die Ausfüllung des Formulars</t>
-  </si>
-  <si>
-    <t>BDEW</t>
-  </si>
-  <si>
-    <t>[…]
-Nr. 22
-Prüfschritt
-Entspricht das Bilanzierungsverfahren dem gültigen Bilanzierungsverfahren zur Datenaggregation beim ÜNB?
-Prüfergebnis 
-ja -&gt; 23
-nein -&gt; 23 Code A09
-Hinweis
-Bilanzierungsverfahren nicht gültig
-Nr. 23
-Prüfschritt
-Wird die Marktlokation auf grundlage von profilen bilanziert?
-Prüfergebnis
-ja -&gt; 24
-nein -&gt;27
-Nr. 24
-Prüfschritt
-Ist das angegebene normierte Profil zum angegebenen Zeitpunkt für das Bilanzierungsgebiet Bestandteil der Profildefinitionsliste des Netzbetreibers?
-Prüfergebnis 
-ja -&gt; 25
-nein -&gt; 25 Code A10
-Hinweis
-Normiertes Profil liegt nicht vor</t>
-  </si>
-  <si>
-    <t>[…]
-Nr. 22
-Prüfschritt
-Entspricht das Bilanzierungsverfahren dem gültigen Bilanzierungsverfahren zur Datenaggregation beim ÜNB?
-Prüfergebnis 
-ja -&gt; 23
-nein -&gt; 23 Code A09
-Hinweis
-Bilanzierungsverfahren nicht gültig
-Nr. 23
-Prüfschritt
-Ist das angegebene normierte Profil zum angegebenen Zeitpunkt für das Bilanzierungsgebiet Bestandteil der Profildefinitionsliste des Netzbetreibers?
-Prüfergebnis 
-ja -&gt; 25
-nein -&gt; 25 Code A10
-Hinweis
-Normiertes Profil liegt nicht vor</t>
-  </si>
-  <si>
-    <t>Die neue Frage (23) ist erforderlich, damit die nächsten Fragen in der richtigen Reihenfolge erfolgen.</t>
-  </si>
-  <si>
-    <t>E_0104_Listeninhalt prüfen</t>
-  </si>
-  <si>
-    <t>E_0105_Listeninhalt prüfen</t>
-  </si>
-  <si>
-    <t>E_0406_Netznutzungsrechnung prüfen</t>
-  </si>
-  <si>
-    <t>E_0407_erneut Netznutzungsabrechnung prüfen</t>
-  </si>
-  <si>
-    <t>E_0450_Information prüfen</t>
-  </si>
-  <si>
-    <t>E_0459_Prüfen, ob Antwort auf Stornierung erforderlich</t>
-  </si>
-  <si>
-    <t>G_0001_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>G_0002_Antwort auf Änderungsmeldung zur Zuordnungsliste-Gas</t>
-  </si>
-  <si>
-    <t>G_0003_Ablehnung Anfrage Stornierung</t>
-  </si>
-  <si>
-    <t>G_0004_Bestätigung Anfrage Stornierung</t>
-  </si>
-  <si>
-    <t>G_0005_Ablehnung Kündigung</t>
-  </si>
-  <si>
-    <t>G_0006_Bestätigung Kündigung</t>
-  </si>
-  <si>
-    <t>G_0007_Ablehnung Abmeldung</t>
-  </si>
-  <si>
-    <t>G_0008_Bestätigung Abmeldung</t>
-  </si>
-  <si>
-    <t>G_0009_Ablehnung Abmeldungsanfrage</t>
-  </si>
-  <si>
-    <t>G_0010_Bestätigung Abmeldungsanfrage</t>
-  </si>
-  <si>
-    <t>G_0011_Ablehnung der Anmeldung</t>
-  </si>
-  <si>
-    <t>G_0012_Bestätigung der Anmeldung</t>
-  </si>
-  <si>
-    <t>G_0013_Bestätigung EOG Anmeldung</t>
-  </si>
-  <si>
-    <t>G_0014_Ablehnung EOG Anmeldung</t>
-  </si>
-  <si>
-    <t>G_0015_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>G_0016_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>G_0017_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>G_0018_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>G_0019_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>G_0022_Antwort auf Änderung der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>G_0023_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>G_0024_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>G_0025_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>G_0026_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>G_0027_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>G_0029_Antwort auf Änderung</t>
-  </si>
-  <si>
-    <t>G_0030_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>G_0031_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0032_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0033_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>G_0034_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0035_Antwort auf Anfrage der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>G_0036_Ablehnung der Anfrage der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>G_0038_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0039_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>G_0040_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0042_Ablehnung Anfrage</t>
-  </si>
-  <si>
-    <t>G_0043_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0044_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0045_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0046_Ablehnung Anfrage</t>
-  </si>
-  <si>
-    <t>G_0047_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0048_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>G_0049_ORDRSP_Ablehnung der Anforderung von Stammdaten</t>
-  </si>
-  <si>
-    <t>G_0050_ORDRSP_Ablehnung der Anforderung von Messwerten</t>
-  </si>
-  <si>
-    <t>G_0051_Ablehnung Kündigung MSB</t>
-  </si>
-  <si>
-    <t>G_0052_Bestätigung Kündigung MSB</t>
-  </si>
-  <si>
-    <t>G_0053_Ablehnung Anmeldung MSB</t>
-  </si>
-  <si>
-    <t>G_0054_Bestätigung Anmeldung MSB</t>
-  </si>
-  <si>
-    <t>G_0055_Statusmeldung</t>
-  </si>
-  <si>
-    <t>G_0057_Ablehnung Ende MSB</t>
-  </si>
-  <si>
-    <t>G_0058_Bestätigung Ende MSB</t>
-  </si>
-  <si>
-    <t>G_0059_Ankündigung zum Eigenausbau</t>
-  </si>
-  <si>
-    <t>G_0060_Mitteilung, kein Eigenausbau MSBA</t>
-  </si>
-  <si>
-    <t>G_0061_ORDRSP Bestellbestätigung</t>
-  </si>
-  <si>
-    <t>G_0062_ORDRSP Ablehnung der Änderung an LF</t>
-  </si>
-  <si>
-    <t>G_0063_ORDRSP Ablehnung der Änderung an NB</t>
-  </si>
-  <si>
-    <t>G_0064_ORDRSP Auftragsbestätigung an LF</t>
-  </si>
-  <si>
-    <t>G_0065_ORDRSP Auftragsbestätigung an NB</t>
-  </si>
-  <si>
-    <t>G_0066_ORDRSP Ablehnung der Reklamation</t>
-  </si>
-  <si>
-    <t>G_0067_Bestätigung Abmeldung von NB</t>
-  </si>
-  <si>
-    <t>G_0068_Ablehnung Abmeldung von NB</t>
-  </si>
-  <si>
-    <t>G_0069_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>G_0070_Bestätigung Verpflichtungsanfrage</t>
-  </si>
-  <si>
-    <t>G_0071_Ablehnung Verpflichtungsanfrage</t>
-  </si>
-  <si>
-    <t>G_0072_ORDRSP Fortführungsbestätigung MSBA</t>
-  </si>
-  <si>
-    <t>G_0073_ORDRSP Ablehnung</t>
-  </si>
-  <si>
-    <t>G_0074_ORDRSP Ablehnung der Bestellung</t>
-  </si>
-  <si>
-    <t>G_0075_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>G_0076_ORDRSP Mitteilung einer gescheiterten Ablesung</t>
-  </si>
-  <si>
-    <t>G_0077_Mitteilung einer gescheiterten Ablesung</t>
-  </si>
-  <si>
-    <t>G_0078_ORDRSP_Ablehnung der Anforderung</t>
-  </si>
-  <si>
-    <t>G_0079_ Kapazitätsrechnung prüfen</t>
-  </si>
-  <si>
-    <t>G_0080_aggregierte Menge und Abrechnungszeitraum prüfen</t>
-  </si>
-  <si>
-    <t>G_0081_Netznutzungsrechnung prüfen</t>
-  </si>
-  <si>
-    <t>G_0082_ORDRSP_Ablehnung der Anforderung von Messwerten</t>
-  </si>
-  <si>
-    <t>G_0083_Ablehnung der Rechnung vom NB an den MSBA</t>
-  </si>
-  <si>
-    <t>G_0084_Ablehnung der Rechnung vom MSBN an den MSBA</t>
-  </si>
-  <si>
-    <t>G_0085_Ablehnung der Stornorechnung</t>
-  </si>
-  <si>
-    <t>G_0086_Ablehnung der Stornorechnung</t>
-  </si>
-  <si>
-    <t>G_0087_Ablehnung der Stornorechnung</t>
-  </si>
-  <si>
-    <t>G_0088_Ablehnung der Stornorechnung (MMMA NB an MGV)</t>
-  </si>
-  <si>
-    <t>GS_001_Ablehnung auf Stammdaten zur verbrauchenden Marktlokation</t>
-  </si>
-  <si>
-    <t>GS_002_MehrMinderMengen-Rechnung prüfen</t>
-  </si>
-  <si>
-    <t>GS_004_Ablehnung der Stornorechnung (aus Prozessschritt 5 MMMA NB an LF)</t>
-  </si>
-  <si>
-    <t>GS_005_Ablehnung der Stornorechnung (aus Prozessschritt 7 MMMA NB an LF)</t>
-  </si>
-  <si>
-    <t>S_0003_Bestätigung EOG Anmeldung</t>
-  </si>
-  <si>
-    <t>S_0004_Ablehnung EOG Anmeldung</t>
-  </si>
-  <si>
-    <t>S_0005_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0006_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0007_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0008_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0009_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0010_Antwort auf Änderung vom NB</t>
-  </si>
-  <si>
-    <t>S_0013_Antwort auf Änderung der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>S_0014_Antwort auf Änderung der Lokationsbündelstruktur</t>
-  </si>
-  <si>
-    <t>S_0015_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>S_0016_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>S_0017_Antwort auf Änderung vom LF</t>
-  </si>
-  <si>
-    <t>S_0018_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>S_0019_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>S_0020_Antwort auf Änderung vom MSB</t>
-  </si>
-  <si>
-    <t>S_0021_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0022_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0023_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0024_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>S_0025_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0026_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0027_Ablehnung der Anfrage der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>S_0028_Antwort auf Anfrage der Lokationsbündelstruktur</t>
-  </si>
-  <si>
-    <t>S_0029_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0030_Ablehnung Anfrage</t>
-  </si>
-  <si>
-    <t>S_0031_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0032_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0033_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>S_0034_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0035_Ablehnung Anfrage</t>
-  </si>
-  <si>
-    <t>S_0036_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0037_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>S_0038_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0039_Antwort auf Änderung</t>
-  </si>
-  <si>
-    <t>S_0040_Antwort auf Änderung</t>
-  </si>
-  <si>
-    <t>S_0041_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0043_ORDRSP_Ablehnung der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0044_ORDRSP_Ablehnung der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0045_Bestätigung Kündigung</t>
-  </si>
-  <si>
-    <t>S_0046_Ablehnung Kündigung</t>
-  </si>
-  <si>
-    <t>S_0047_Bestätigung Abmeldungsanfrage</t>
-  </si>
-  <si>
-    <t>S_0048_Ablehnung Abmeldungsanfrage</t>
-  </si>
-  <si>
-    <t>S_0049_Bestätigung Anmeldung</t>
-  </si>
-  <si>
-    <t>S_0050_Bestätigung Anmeldung Neuanl. u. LW m. Trbild. b. N-EE+N-KWKG</t>
-  </si>
-  <si>
-    <t>S_0051_Ablehnung Anmeldung</t>
-  </si>
-  <si>
-    <t>S_0052_Ablehnung Abmeldung</t>
-  </si>
-  <si>
-    <t>S_0054_Ablehnung Kündigung MSB</t>
-  </si>
-  <si>
-    <t>S_0055_Bestätigung Anmeldung MSB</t>
-  </si>
-  <si>
-    <t>S_0056_Ablehnung Anmeldung MSB</t>
-  </si>
-  <si>
-    <t>S_0057_Statusmeldung</t>
-  </si>
-  <si>
-    <t>S_0059_Bestätigung Ende MSB</t>
-  </si>
-  <si>
-    <t>S_0060_Ablehnung Ende MSB</t>
-  </si>
-  <si>
-    <t>S_0061_ORDRSP Fortführungsbestätigung MSBA</t>
-  </si>
-  <si>
-    <t>S_0062_ORDRSP Ablehnung</t>
-  </si>
-  <si>
-    <t>S_0063_Bestätigung Verpflichtungsanfrage</t>
-  </si>
-  <si>
-    <t>S_0064_Ablehnung Verpflichtungsanfrage</t>
-  </si>
-  <si>
-    <t>S_0065_Ankündigung zum Eigenausbau</t>
-  </si>
-  <si>
-    <t>S_0066_Mitteilung, kein Eigenausbau MSBA</t>
-  </si>
-  <si>
-    <t>S_0067_ORDRSP Bestellbestätigung</t>
-  </si>
-  <si>
-    <t>S_0068_ORDRSP Abl. der Bestellung</t>
-  </si>
-  <si>
-    <t>S_0073_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0074_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0075_ORDRSP Abl. der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0076_ORDRSP Ablehnung der Reklamation</t>
-  </si>
-  <si>
-    <t>S_0077_ORDRSP Ablehnung der Reklamation</t>
-  </si>
-  <si>
-    <t>S_0078_ORDRSP Ablehnung der Reklamation</t>
-  </si>
-  <si>
-    <t>S_0079_ORDRSP Ablehnung der Reklamation</t>
-  </si>
-  <si>
-    <t>S_0080_Ablehnung auf Stammdaten zur erzeugenden Marktlokation</t>
-  </si>
-  <si>
-    <t>S_0086_Bestätigung Anfrage Stornierung</t>
-  </si>
-  <si>
-    <t>S_0087_Ablehnung Anfrage Stornierung</t>
-  </si>
-  <si>
-    <t>S_0088_Bestätigung Abmeldung</t>
-  </si>
-  <si>
-    <t>S_0090_Bestätigung Kündigung MSBS</t>
-  </si>
-  <si>
-    <t>S_0091_Antwort auf Stammdatenänderung</t>
-  </si>
-  <si>
-    <t>S_0092_ORDRSP Ablehnung der Anforderung</t>
-  </si>
-  <si>
-    <t>S_0093_ORDRSP Bestätigung der Anforderung zum Beenden des Abos zur Stammdaten- bzw. Messwertübermittlung</t>
-  </si>
-  <si>
-    <t>S_0094_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0098_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>S_0099_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0100_Ablehnung der Anfrage</t>
-  </si>
-  <si>
-    <t>S_0101_Antwort auf Anfrage der Marktlokationsstruktur</t>
-  </si>
-  <si>
-    <t>S_0102_Antwort auf Anfrage</t>
-  </si>
-  <si>
-    <t>S_0103_Netznutzungsrechnung prüfen</t>
-  </si>
-  <si>
-    <t>S_0104_erneut Netznutzungsrechnung prüfen</t>
-  </si>
-  <si>
-    <t>S_0106_ Rechnung verarbeiten</t>
-  </si>
-  <si>
-    <t>S_0107_Abrechnung von Dienstleistungen</t>
-  </si>
-  <si>
-    <t>S_0108_Weitere Bearbeitung prüfen</t>
-  </si>
-  <si>
-    <t>S_0109_Nichtzahlungsavis prüfen</t>
-  </si>
-  <si>
-    <t>S_0110_Prüfen, ob Antwort auf Stornierung erforderlich</t>
-  </si>
-  <si>
-    <t>S_0111_Prüfen, ob Antwort auf Stornierung erforderlich</t>
   </si>
 </sst>
 </file>
@@ -1905,27 +1905,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24604197-F8EF-46B1-B2CD-541043B1C494}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="50.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="44.25" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1955,13 +1955,13 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.5">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="7" spans="1:4" ht="217.5" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>6</v>
+        <v>345</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -1988,81 +1988,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B43C9C9-CC5E-422F-81E2-6BCD41742AA5}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" style="6" customWidth="1"/>
-    <col min="6" max="7" width="78.7109375" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="41.26953125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="78.7265625" customWidth="1"/>
+    <col min="8" max="8" width="36.1796875" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="47.25">
+    <row r="1" spans="1:10" ht="31">
       <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="391.5">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="405">
-      <c r="A2" s="18" t="s">
-        <v>17</v>
-      </c>
       <c r="B2" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="19">
         <v>93</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2770,1624 +2770,1624 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="86.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="86.54296875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2" ht="29">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" s="20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="305" spans="2:2">
       <c r="B305" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="306" spans="2:2">
       <c r="B306" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="307" spans="2:2">
       <c r="B307" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="308" spans="2:2">
       <c r="B308" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="309" spans="2:2">
       <c r="B309" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="310" spans="2:2">
       <c r="B310" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="311" spans="2:2">
       <c r="B311" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="312" spans="2:2">
       <c r="B312" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="313" spans="2:2">
       <c r="B313" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="314" spans="2:2">
       <c r="B314" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="315" spans="2:2">
       <c r="B315" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="316" spans="2:2">
       <c r="B316" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="317" spans="2:2">
       <c r="B317" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="318" spans="2:2">
       <c r="B318" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="319" spans="2:2">
       <c r="B319" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="320" spans="2:2">
       <c r="B320" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="321" spans="2:2">
       <c r="B321" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="322" spans="2:2">
       <c r="B322" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>